<commit_message>
Project code updated - Abeer
</commit_message>
<xml_diff>
--- a/abeer_utils/testData.xlsx
+++ b/abeer_utils/testData.xlsx
@@ -460,7 +460,7 @@
         <v>Last</v>
       </c>
       <c r="D2" t="str">
-        <v>0391</v>
+        <v>422</v>
       </c>
     </row>
   </sheetData>
@@ -490,7 +490,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>First0391</v>
+        <v>First422</v>
       </c>
       <c r="B2" t="str">
         <v>Password_123</v>
@@ -538,7 +538,7 @@
         <v>123</v>
       </c>
       <c r="B2" t="str">
-        <v>2027-28-02</v>
+        <v>2027-02-02</v>
       </c>
       <c r="C2" t="str">
         <v>Bangladeshi</v>

</xml_diff>